<commit_message>
Se agrega espera para validar si aparece modal y cerrarlo y se agregan comentarios
</commit_message>
<xml_diff>
--- a/TerminosBusqueda.xlsx
+++ b/TerminosBusqueda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\semilleroPruebas\Proyectos\Reto1_bestBuy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8539BBE2-D75F-4E7E-851C-54F7397A0C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD3B058-D199-4399-9C62-624C3436194E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -48,13 +48,13 @@
     <t>Titulo_Producto</t>
   </si>
   <si>
-    <t>Unagi Model One E350 Foldable Electric Scooter w/15 mi Max Operating Range &amp; 15.5 mph Max Speed Grey 1003110350 - Best Buy</t>
-  </si>
-  <si>
     <t>vacuum robot</t>
   </si>
   <si>
-    <t>iRobot Roomba i3+ (3550) Wi-Fi Connected Self Emptying Robot Vacuum Neutral i355020 - Best Buy</t>
+    <t>Hover-1 Alpha Foldable Electric Scooter w/12 mi Max Operating Range &amp; 17.4 mph Max Speed Black H1-ALPHA-BLK - Best Buy</t>
+  </si>
+  <si>
+    <t>BISSELL SpinWave Wet and Dry Robotic Vacuum Pearl White 2859 - Best Buy</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -427,7 +427,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Se organiza escenario en el feature y en el stepdefinition
</commit_message>
<xml_diff>
--- a/TerminosBusqueda.xlsx
+++ b/TerminosBusqueda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\semilleroPruebas\Proyectos\Reto1_bestBuy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD3B058-D199-4399-9C62-624C3436194E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF2AF53-B8E7-4C8F-B5A5-293D8A312FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>pc gamer</t>
   </si>
@@ -48,13 +48,7 @@
     <t>Titulo_Producto</t>
   </si>
   <si>
-    <t>vacuum robot</t>
-  </si>
-  <si>
     <t>Hover-1 Alpha Foldable Electric Scooter w/12 mi Max Operating Range &amp; 17.4 mph Max Speed Black H1-ALPHA-BLK - Best Buy</t>
-  </si>
-  <si>
-    <t>BISSELL SpinWave Wet and Dry Robotic Vacuum Pearl White 2859 - Best Buy</t>
   </si>
 </sst>
 </file>
@@ -381,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +408,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -423,14 +417,6 @@
       </c>
       <c r="B4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>